<commit_message>
Schematic: dokumentation + obsolet switch changed
</commit_message>
<xml_diff>
--- a/production/BOM/BOM_ZumoComSystem.xlsx
+++ b/production/BOM/BOM_ZumoComSystem.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26026"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27531"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nschneider\Documents\NT_Projekte\ZumoCom\Repository\Electronic\Production\BOM\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nschneider\Documents\NT_Projekte\ZumoComSystemHW\production\BOM\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FC6BC83C-A3FF-437A-A140-4B5EC36030F5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B63656CF-F22E-4901-8348-C667A50496C9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -25,14 +25,11 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="264" uniqueCount="222">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="264" uniqueCount="220">
   <si>
     <t>ZumoComSystem</t>
   </si>
   <si>
-    <t>MLL1200S</t>
-  </si>
-  <si>
     <t>Bourns Inc.</t>
   </si>
   <si>
@@ -267,12 +264,6 @@
     <t xml:space="preserve">    SW1</t>
   </si>
   <si>
-    <t xml:space="preserve">TE Connectivity / P&amp;B </t>
-  </si>
-  <si>
-    <t xml:space="preserve">MLL1200S </t>
-  </si>
-  <si>
     <t>TL3342F260QG</t>
   </si>
   <si>
@@ -651,9 +642,6 @@
     <t>User_Button</t>
   </si>
   <si>
-    <t>&gt;  SW2-SW5</t>
-  </si>
-  <si>
     <t>SW_Push</t>
   </si>
   <si>
@@ -691,6 +679,12 @@
   </si>
   <si>
     <t>v2.0</t>
+  </si>
+  <si>
+    <t>&gt;  SW2-SW5, SW7</t>
+  </si>
+  <si>
+    <t>EG1257</t>
   </si>
 </sst>
 </file>
@@ -1085,8 +1079,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A2:H76"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="K6" sqref="K6"/>
+    <sheetView tabSelected="1" topLeftCell="A9" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="J61" sqref="J61"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1108,10 +1102,10 @@
         <v>0</v>
       </c>
       <c r="D2" s="6" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
       <c r="E2" s="7" t="s">
-        <v>221</v>
+        <v>217</v>
       </c>
     </row>
     <row r="3" spans="1:8" ht="21" x14ac:dyDescent="0.35">
@@ -1119,30 +1113,30 @@
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
+        <v>88</v>
+      </c>
+      <c r="B4" t="s">
+        <v>89</v>
+      </c>
+      <c r="C4" t="s">
+        <v>90</v>
+      </c>
+      <c r="D4" t="s">
         <v>91</v>
       </c>
-      <c r="B4" t="s">
-        <v>92</v>
-      </c>
-      <c r="C4" t="s">
-        <v>93</v>
-      </c>
-      <c r="D4" t="s">
-        <v>94</v>
-      </c>
       <c r="E4" s="3" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
       <c r="D5" s="3">
         <v>1043</v>
@@ -1153,16 +1147,16 @@
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
       <c r="B6" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="C6" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="C6" s="3" t="s">
+      <c r="D6" s="4" t="s">
         <v>16</v>
-      </c>
-      <c r="D6" s="4" t="s">
-        <v>17</v>
       </c>
       <c r="E6" s="5">
         <v>3</v>
@@ -1171,16 +1165,16 @@
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="D7" s="4" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="E7" s="5">
         <v>3</v>
@@ -1189,16 +1183,16 @@
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
       <c r="B8" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="C8" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="D8" s="4" t="s">
         <v>20</v>
-      </c>
-      <c r="C8" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="D8" s="4" t="s">
-        <v>21</v>
       </c>
       <c r="E8" s="5">
         <v>1</v>
@@ -1207,16 +1201,16 @@
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
       <c r="B9" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="C9" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="D9" s="4" t="s">
         <v>18</v>
-      </c>
-      <c r="C9" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="D9" s="4" t="s">
-        <v>19</v>
       </c>
       <c r="E9" s="5">
         <v>1</v>
@@ -1225,16 +1219,16 @@
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="s">
-        <v>139</v>
+        <v>136</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="D10" s="4" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="E10" s="5">
         <v>1</v>
@@ -1243,16 +1237,16 @@
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" s="3" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D11" s="4" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="E11" s="5">
         <v>1</v>
@@ -1261,16 +1255,16 @@
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" s="3" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="C12" s="3" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
       <c r="D12" s="4" t="s">
-        <v>143</v>
+        <v>140</v>
       </c>
       <c r="E12" s="5">
         <v>2</v>
@@ -1279,16 +1273,16 @@
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" s="3" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
       <c r="C13" s="3" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D13" s="4" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="E13" s="5">
         <v>1</v>
@@ -1297,16 +1291,16 @@
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" s="3" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="C14" s="3" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D14" s="4" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="E14" s="5">
         <v>1</v>
@@ -1315,16 +1309,16 @@
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15" s="3" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
       <c r="C15" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="D15" s="4" t="s">
         <v>39</v>
-      </c>
-      <c r="D15" s="4" t="s">
-        <v>40</v>
       </c>
       <c r="E15" s="5">
         <v>1</v>
@@ -1333,16 +1327,16 @@
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16" s="3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B16" s="3" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
       <c r="C16" s="3" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
       <c r="D16" s="4" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
       <c r="E16" s="5">
         <v>1</v>
@@ -1351,16 +1345,16 @@
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A17" s="3" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B17" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="C17" s="3" t="s">
+        <v>124</v>
+      </c>
+      <c r="D17" s="4" t="s">
         <v>35</v>
-      </c>
-      <c r="C17" s="3" t="s">
-        <v>127</v>
-      </c>
-      <c r="D17" s="4" t="s">
-        <v>36</v>
       </c>
       <c r="E17" s="5">
         <v>1</v>
@@ -1369,16 +1363,16 @@
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A18" s="3" t="s">
-        <v>147</v>
+        <v>144</v>
       </c>
       <c r="B18" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="C18" s="3" t="s">
+        <v>124</v>
+      </c>
+      <c r="D18" s="4" t="s">
         <v>32</v>
-      </c>
-      <c r="C18" s="3" t="s">
-        <v>127</v>
-      </c>
-      <c r="D18" s="4" t="s">
-        <v>33</v>
       </c>
       <c r="E18" s="5">
         <v>1</v>
@@ -1387,16 +1381,16 @@
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A19" s="3" t="s">
-        <v>148</v>
+        <v>145</v>
       </c>
       <c r="B19" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="C19" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="C19" s="3" t="s">
-        <v>31</v>
-      </c>
       <c r="D19" s="4" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="E19" s="5">
         <v>6</v>
@@ -1405,16 +1399,16 @@
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A20" s="3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B20" s="3" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
       <c r="C20" s="3" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
       <c r="D20" s="4" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
       <c r="E20" s="5">
         <v>1</v>
@@ -1423,16 +1417,16 @@
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A21" s="3" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B21" s="3" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
       <c r="C21" s="3" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D21" s="4" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
       <c r="E21" s="5">
         <v>1</v>
@@ -1441,16 +1435,16 @@
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A22" s="3" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B22" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="C22" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="C22" s="3" t="s">
+      <c r="D22" s="4" t="s">
         <v>28</v>
-      </c>
-      <c r="D22" s="4" t="s">
-        <v>29</v>
       </c>
       <c r="E22" s="5">
         <v>1</v>
@@ -1459,16 +1453,16 @@
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A23" s="3" t="s">
-        <v>154</v>
+        <v>151</v>
       </c>
       <c r="B23" s="3" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C23" s="3" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
       <c r="D23" s="4" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E23" s="5">
         <v>1</v>
@@ -1477,16 +1471,16 @@
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A24" s="3" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
       <c r="B24" s="3" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C24" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="D24" s="4" t="s">
         <v>24</v>
-      </c>
-      <c r="D24" s="4" t="s">
-        <v>25</v>
       </c>
       <c r="E24" s="5">
         <v>1</v>
@@ -1495,16 +1489,16 @@
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A25" s="3" t="s">
-        <v>156</v>
+        <v>153</v>
       </c>
       <c r="B25" s="3" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
       <c r="C25" s="3" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D25" s="4" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
       <c r="E25" s="5">
         <v>1</v>
@@ -1513,16 +1507,16 @@
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A26" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="B26" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="B26" s="3" t="s">
-        <v>42</v>
-      </c>
       <c r="C26" s="3" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D26" s="4" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="E26" s="5">
         <v>1</v>
@@ -1531,16 +1525,16 @@
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A27" s="3" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
       <c r="B27" s="3" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="C27" s="3" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
       <c r="D27" s="4" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="E27" s="5">
         <v>1</v>
@@ -1549,16 +1543,16 @@
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A28" s="3" t="s">
+        <v>157</v>
+      </c>
+      <c r="B28" s="4" t="s">
+        <v>158</v>
+      </c>
+      <c r="C28" s="3" t="s">
+        <v>159</v>
+      </c>
+      <c r="D28" s="4" t="s">
         <v>160</v>
-      </c>
-      <c r="B28" s="4" t="s">
-        <v>161</v>
-      </c>
-      <c r="C28" s="3" t="s">
-        <v>162</v>
-      </c>
-      <c r="D28" s="4" t="s">
-        <v>163</v>
       </c>
       <c r="E28" s="5">
         <v>1</v>
@@ -1567,16 +1561,16 @@
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A29" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="B29" s="3" t="s">
         <v>43</v>
       </c>
-      <c r="B29" s="3" t="s">
+      <c r="C29" s="3" t="s">
         <v>44</v>
       </c>
-      <c r="C29" s="3" t="s">
-        <v>45</v>
-      </c>
       <c r="D29" s="4" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="E29" s="5">
         <v>1</v>
@@ -1585,16 +1579,16 @@
     </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A30" s="3" t="s">
-        <v>164</v>
+        <v>161</v>
       </c>
       <c r="B30" s="3" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="C30" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="D30" s="4" t="s">
         <v>48</v>
-      </c>
-      <c r="D30" s="4" t="s">
-        <v>49</v>
       </c>
       <c r="E30" s="5">
         <v>2</v>
@@ -1603,16 +1597,16 @@
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A31" s="3" t="s">
-        <v>165</v>
+        <v>162</v>
       </c>
       <c r="B31" s="3" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C31" s="3" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D31" s="4" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
       <c r="E31" s="5">
         <v>1</v>
@@ -1621,16 +1615,16 @@
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A32" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="B32" s="3" t="s">
         <v>50</v>
       </c>
-      <c r="B32" s="3" t="s">
-        <v>51</v>
-      </c>
       <c r="C32" s="3" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D32" s="4" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="E32" s="5">
         <v>1</v>
@@ -1639,16 +1633,16 @@
     </row>
     <row r="33" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A33" s="3" t="s">
-        <v>167</v>
+        <v>164</v>
       </c>
       <c r="B33" s="3" t="s">
-        <v>168</v>
+        <v>165</v>
       </c>
       <c r="C33" s="3" t="s">
-        <v>169</v>
+        <v>166</v>
       </c>
       <c r="D33" s="4" t="s">
-        <v>168</v>
+        <v>165</v>
       </c>
       <c r="E33" s="5">
         <v>1</v>
@@ -1657,16 +1651,16 @@
     </row>
     <row r="34" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A34" s="3" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B34" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="C34" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="D34" s="4" t="s">
         <v>46</v>
-      </c>
-      <c r="C34" s="3" t="s">
-        <v>45</v>
-      </c>
-      <c r="D34" s="4" t="s">
-        <v>47</v>
       </c>
       <c r="E34" s="5">
         <v>1</v>
@@ -1675,16 +1669,16 @@
     </row>
     <row r="35" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A35" s="3" t="s">
-        <v>170</v>
+        <v>167</v>
       </c>
       <c r="B35" s="3" t="s">
-        <v>171</v>
+        <v>168</v>
       </c>
       <c r="C35" s="3" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="D35" s="4" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="E35" s="5">
         <v>2</v>
@@ -1693,16 +1687,16 @@
     </row>
     <row r="36" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A36" s="3" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B36" s="3" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
       <c r="C36" s="3" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="D36" s="4" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="E36" s="5">
         <v>1</v>
@@ -1710,16 +1704,16 @@
     </row>
     <row r="37" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A37" s="3" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B37" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="C37" s="3" t="s">
         <v>62</v>
       </c>
-      <c r="C37" s="3" t="s">
-        <v>63</v>
-      </c>
       <c r="D37" s="4" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="E37" s="5">
         <v>1</v>
@@ -1728,16 +1722,16 @@
     </row>
     <row r="38" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A38" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="B38" s="3" t="s">
         <v>57</v>
       </c>
-      <c r="B38" s="3" t="s">
-        <v>58</v>
-      </c>
       <c r="C38" s="3" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D38" s="3" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="E38" s="5">
         <v>2</v>
@@ -1746,16 +1740,16 @@
     </row>
     <row r="39" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A39" s="3" t="s">
+        <v>169</v>
+      </c>
+      <c r="B39" s="3" t="s">
+        <v>170</v>
+      </c>
+      <c r="C39" s="3" t="s">
+        <v>171</v>
+      </c>
+      <c r="D39" s="3" t="s">
         <v>172</v>
-      </c>
-      <c r="B39" s="3" t="s">
-        <v>173</v>
-      </c>
-      <c r="C39" s="3" t="s">
-        <v>174</v>
-      </c>
-      <c r="D39" s="3" t="s">
-        <v>175</v>
       </c>
       <c r="E39" s="5">
         <v>1</v>
@@ -1763,16 +1757,16 @@
     </row>
     <row r="40" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A40" s="3" t="s">
-        <v>176</v>
+        <v>173</v>
       </c>
       <c r="B40" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="C40" s="3" t="s">
         <v>59</v>
       </c>
-      <c r="C40" s="3" t="s">
+      <c r="D40" s="3" t="s">
         <v>60</v>
-      </c>
-      <c r="D40" s="3" t="s">
-        <v>61</v>
       </c>
       <c r="E40" s="5">
         <v>2</v>
@@ -1780,16 +1774,16 @@
     </row>
     <row r="41" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A41" s="3" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
       <c r="B41" s="3" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="C41" s="3" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="D41" s="3" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
       <c r="E41" s="5">
         <v>1</v>
@@ -1797,16 +1791,16 @@
     </row>
     <row r="42" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A42" s="3" t="s">
-        <v>177</v>
+        <v>174</v>
       </c>
       <c r="B42" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="C42" s="3" t="s">
         <v>64</v>
       </c>
-      <c r="C42" s="3" t="s">
+      <c r="D42" s="3" t="s">
         <v>65</v>
-      </c>
-      <c r="D42" s="3" t="s">
-        <v>66</v>
       </c>
       <c r="E42" s="5">
         <v>8</v>
@@ -1814,16 +1808,16 @@
     </row>
     <row r="43" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A43" s="3" t="s">
-        <v>178</v>
+        <v>175</v>
       </c>
       <c r="B43" s="3">
         <v>300</v>
       </c>
       <c r="C43" s="3" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D43" s="3" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="E43" s="5">
         <v>1</v>
@@ -1831,16 +1825,16 @@
     </row>
     <row r="44" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A44" s="3" t="s">
-        <v>179</v>
+        <v>176</v>
       </c>
       <c r="B44" s="3">
         <v>100</v>
       </c>
       <c r="C44" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D44" s="3" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
       <c r="E44" s="5">
         <v>2</v>
@@ -1848,16 +1842,16 @@
     </row>
     <row r="45" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A45" s="3" t="s">
-        <v>180</v>
+        <v>177</v>
       </c>
       <c r="B45" s="3">
         <v>620</v>
       </c>
       <c r="C45" s="3" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
       <c r="D45" s="3" t="s">
-        <v>181</v>
+        <v>178</v>
       </c>
       <c r="E45" s="5">
         <v>3</v>
@@ -1865,16 +1859,16 @@
     </row>
     <row r="46" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A46" s="3" t="s">
-        <v>182</v>
+        <v>179</v>
       </c>
       <c r="B46" s="3">
         <v>0</v>
       </c>
       <c r="C46" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D46" s="3" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="E46" s="5">
         <v>3</v>
@@ -1882,16 +1876,16 @@
     </row>
     <row r="47" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A47" s="3" t="s">
-        <v>183</v>
+        <v>180</v>
       </c>
       <c r="B47" s="3">
         <v>470</v>
       </c>
       <c r="C47" s="3" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="D47" s="3" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="E47" s="5">
         <v>2</v>
@@ -1899,16 +1893,16 @@
     </row>
     <row r="48" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A48" s="3" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="B48" s="3" t="s">
-        <v>184</v>
+        <v>181</v>
       </c>
       <c r="C48" s="3" t="s">
-        <v>185</v>
+        <v>182</v>
       </c>
       <c r="D48" s="3" t="s">
-        <v>186</v>
+        <v>183</v>
       </c>
       <c r="E48" s="5">
         <v>1</v>
@@ -1916,16 +1910,16 @@
     </row>
     <row r="49" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A49" s="3" t="s">
+        <v>184</v>
+      </c>
+      <c r="B49" s="3" t="s">
+        <v>185</v>
+      </c>
+      <c r="C49" s="3" t="s">
+        <v>186</v>
+      </c>
+      <c r="D49" s="3" t="s">
         <v>187</v>
-      </c>
-      <c r="B49" s="3" t="s">
-        <v>188</v>
-      </c>
-      <c r="C49" s="3" t="s">
-        <v>189</v>
-      </c>
-      <c r="D49" s="3" t="s">
-        <v>190</v>
       </c>
       <c r="E49" s="5">
         <v>1</v>
@@ -1933,16 +1927,16 @@
     </row>
     <row r="50" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A50" s="3" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
       <c r="B50" s="3">
         <v>0</v>
       </c>
       <c r="C50" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D50" s="3" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="E50" s="5">
         <v>1</v>
@@ -1950,16 +1944,16 @@
     </row>
     <row r="51" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A51" s="3" t="s">
-        <v>191</v>
+        <v>188</v>
       </c>
       <c r="B51" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="C51" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="D51" s="3" t="s">
         <v>72</v>
-      </c>
-      <c r="C51" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="D51" s="3" t="s">
-        <v>73</v>
       </c>
       <c r="E51" s="5">
         <v>1</v>
@@ -1967,16 +1961,16 @@
     </row>
     <row r="52" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A52" s="3" t="s">
-        <v>192</v>
+        <v>189</v>
       </c>
       <c r="B52" s="3" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
       <c r="C52" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="D52" s="3" t="s">
         <v>65</v>
-      </c>
-      <c r="D52" s="3" t="s">
-        <v>66</v>
       </c>
       <c r="E52" s="5">
         <v>1</v>
@@ -1984,16 +1978,16 @@
     </row>
     <row r="53" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A53" s="3" t="s">
-        <v>193</v>
+        <v>190</v>
       </c>
       <c r="B53" s="3" t="s">
+        <v>75</v>
+      </c>
+      <c r="C53" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="D53" s="3" t="s">
         <v>76</v>
-      </c>
-      <c r="C53" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="D53" s="3" t="s">
-        <v>77</v>
       </c>
       <c r="E53" s="5">
         <v>1</v>
@@ -2001,16 +1995,16 @@
     </row>
     <row r="54" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A54" s="3" t="s">
-        <v>194</v>
+        <v>191</v>
       </c>
       <c r="B54" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="C54" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="D54" s="3" t="s">
         <v>69</v>
-      </c>
-      <c r="C54" s="3" t="s">
-        <v>65</v>
-      </c>
-      <c r="D54" s="3" t="s">
-        <v>70</v>
       </c>
       <c r="E54" s="5">
         <v>1</v>
@@ -2018,16 +2012,16 @@
     </row>
     <row r="55" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A55" s="3" t="s">
-        <v>195</v>
+        <v>192</v>
       </c>
       <c r="B55" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="C55" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="D55" s="3" t="s">
         <v>74</v>
-      </c>
-      <c r="C55" s="3" t="s">
-        <v>65</v>
-      </c>
-      <c r="D55" s="3" t="s">
-        <v>75</v>
       </c>
       <c r="E55" s="5">
         <v>2</v>
@@ -2035,16 +2029,16 @@
     </row>
     <row r="56" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A56" s="3" t="s">
+        <v>193</v>
+      </c>
+      <c r="B56" s="3" t="s">
+        <v>194</v>
+      </c>
+      <c r="C56" s="3" t="s">
+        <v>195</v>
+      </c>
+      <c r="D56" s="3" t="s">
         <v>196</v>
-      </c>
-      <c r="B56" s="3" t="s">
-        <v>197</v>
-      </c>
-      <c r="C56" s="3" t="s">
-        <v>198</v>
-      </c>
-      <c r="D56" s="3" t="s">
-        <v>199</v>
       </c>
       <c r="E56" s="5">
         <v>1</v>
@@ -2052,16 +2046,16 @@
     </row>
     <row r="57" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A57" s="3" t="s">
-        <v>200</v>
+        <v>197</v>
       </c>
       <c r="B57" s="3" t="s">
-        <v>201</v>
+        <v>198</v>
       </c>
       <c r="C57" s="3" t="s">
-        <v>198</v>
+        <v>195</v>
       </c>
       <c r="D57" s="3" t="s">
-        <v>202</v>
+        <v>199</v>
       </c>
       <c r="E57" s="5">
         <v>1</v>
@@ -2069,16 +2063,16 @@
     </row>
     <row r="58" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A58" s="3" t="s">
+        <v>200</v>
+      </c>
+      <c r="B58" s="3" t="s">
+        <v>201</v>
+      </c>
+      <c r="C58" s="3" t="s">
+        <v>202</v>
+      </c>
+      <c r="D58" s="3" t="s">
         <v>203</v>
-      </c>
-      <c r="B58" s="3" t="s">
-        <v>204</v>
-      </c>
-      <c r="C58" s="3" t="s">
-        <v>205</v>
-      </c>
-      <c r="D58" s="3" t="s">
-        <v>206</v>
       </c>
       <c r="E58" s="5">
         <v>1</v>
@@ -2086,16 +2080,16 @@
     </row>
     <row r="59" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A59" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="B59" s="3" t="s">
+        <v>204</v>
+      </c>
+      <c r="C59" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="D59" s="3" t="s">
         <v>79</v>
-      </c>
-      <c r="B59" s="3" t="s">
-        <v>207</v>
-      </c>
-      <c r="C59" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="D59" s="3" t="s">
-        <v>82</v>
       </c>
       <c r="E59" s="5">
         <v>1</v>
@@ -2103,33 +2097,33 @@
     </row>
     <row r="60" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A60" s="3" t="s">
-        <v>208</v>
+        <v>218</v>
       </c>
       <c r="B60" s="3" t="s">
-        <v>209</v>
+        <v>205</v>
       </c>
       <c r="C60" s="3" t="s">
-        <v>210</v>
+        <v>206</v>
       </c>
       <c r="D60" s="3" t="s">
-        <v>211</v>
+        <v>207</v>
       </c>
       <c r="E60" s="5">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="61" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A61" s="3" t="s">
-        <v>212</v>
+        <v>208</v>
       </c>
       <c r="B61" s="3" t="s">
-        <v>1</v>
+        <v>219</v>
       </c>
       <c r="C61" s="3" t="s">
-        <v>80</v>
+        <v>2</v>
       </c>
       <c r="D61" s="3" t="s">
-        <v>81</v>
+        <v>219</v>
       </c>
       <c r="E61" s="5">
         <v>1</v>
@@ -2137,16 +2131,16 @@
     </row>
     <row r="62" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A62" s="3" t="s">
-        <v>213</v>
+        <v>209</v>
       </c>
       <c r="B62" s="3" t="s">
-        <v>214</v>
+        <v>210</v>
       </c>
       <c r="C62" s="3" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="D62" s="3" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="E62" s="5">
         <v>4</v>
@@ -2154,16 +2148,16 @@
     </row>
     <row r="63" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A63" s="3" t="s">
-        <v>215</v>
+        <v>211</v>
       </c>
       <c r="B63" s="3" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="C63" s="3" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="D63" s="3" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="E63" s="5">
         <v>2</v>
@@ -2171,16 +2165,16 @@
     </row>
     <row r="64" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A64" s="3" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="B64" s="3" t="s">
-        <v>216</v>
+        <v>212</v>
       </c>
       <c r="C64" s="3" t="s">
-        <v>217</v>
+        <v>213</v>
       </c>
       <c r="D64" s="3" t="s">
-        <v>216</v>
+        <v>212</v>
       </c>
       <c r="E64" s="5">
         <v>1</v>
@@ -2188,16 +2182,16 @@
     </row>
     <row r="65" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A65" s="3" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="B65" s="3" t="s">
-        <v>218</v>
+        <v>214</v>
       </c>
       <c r="C65" s="3" t="s">
-        <v>219</v>
+        <v>215</v>
       </c>
       <c r="D65" s="3" t="s">
-        <v>218</v>
+        <v>214</v>
       </c>
       <c r="E65" s="5">
         <v>1</v>
@@ -2205,16 +2199,16 @@
     </row>
     <row r="66" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A66" s="3" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="B66" s="3" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="C66" s="3" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="D66" s="3" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="E66" s="5">
         <v>1</v>
@@ -2222,16 +2216,16 @@
     </row>
     <row r="67" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A67" s="3" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="B67" s="3" t="s">
-        <v>220</v>
+        <v>216</v>
       </c>
       <c r="C67" s="3" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="D67" s="3" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="E67" s="5">
         <v>1</v>
@@ -2245,13 +2239,13 @@
     </row>
     <row r="69" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A69" s="3" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="B69" s="3" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="C69" s="3" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="D69" s="3">
         <v>100833</v>
@@ -2262,16 +2256,16 @@
     </row>
     <row r="70" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A70" s="3" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="B70" s="3" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="C70" s="3" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D70" s="3" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="E70" s="5">
         <v>1</v>
@@ -2279,16 +2273,16 @@
     </row>
     <row r="71" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A71" s="3" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
       <c r="B71" s="3" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
       <c r="C71" s="3" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D71" s="3" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
       <c r="E71" s="5">
         <v>2</v>

</xml_diff>

<commit_message>
add Pin Socket for CamDroid (J8); rerouted, gerber created
</commit_message>
<xml_diff>
--- a/production/BOM/BOM_ZumoComSystem.xlsx
+++ b/production/BOM/BOM_ZumoComSystem.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27531"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="29328"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nschneider\Documents\NT_Projekte\ZumoComSystemHW\production\BOM\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B63656CF-F22E-4901-8348-C667A50496C9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{78ABEBF1-7825-4B4E-B612-F6FB0BA65D11}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="5085" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="264" uniqueCount="220">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="252" uniqueCount="214">
   <si>
     <t>ZumoComSystem</t>
   </si>
@@ -228,9 +228,6 @@
     <t>RC0603FR-070RL</t>
   </si>
   <si>
-    <t>-</t>
-  </si>
-  <si>
     <t>2.2k</t>
   </si>
   <si>
@@ -363,9 +360,6 @@
     <t>IHLP4040DZER150M5A</t>
   </si>
   <si>
-    <t xml:space="preserve">PMOS_GSD-TSM260P02CX RFG </t>
-  </si>
-  <si>
     <t xml:space="preserve">Taiwan Semiconductor </t>
   </si>
   <si>
@@ -375,9 +369,6 @@
     <t>10k / 0.1%</t>
   </si>
   <si>
-    <t>TP_2P</t>
-  </si>
-  <si>
     <t xml:space="preserve">   J4*, J6*</t>
   </si>
   <si>
@@ -528,12 +519,6 @@
     <t>CUI Devices</t>
   </si>
   <si>
-    <t>&gt;  JP1, JP2</t>
-  </si>
-  <si>
-    <t>SolderJumper_2_Open</t>
-  </si>
-  <si>
     <t xml:space="preserve">    Q4</t>
   </si>
   <si>
@@ -654,15 +639,6 @@
     <t xml:space="preserve">    SW6</t>
   </si>
   <si>
-    <t>&gt;  TP1-TP4</t>
-  </si>
-  <si>
-    <t>TestPoint</t>
-  </si>
-  <si>
-    <t>&gt;  TP5, TP7</t>
-  </si>
-  <si>
     <t>ESP32-S3-WROOM-1</t>
   </si>
   <si>
@@ -685,6 +661,12 @@
   </si>
   <si>
     <t>EG1257</t>
+  </si>
+  <si>
+    <t>PMOS_GSD-TSM260P02CX RFG</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Texas Instruments </t>
   </si>
 </sst>
 </file>
@@ -801,8 +783,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Tabelle1" displayName="Tabelle1" ref="A4:E72" totalsRowShown="0" dataDxfId="5">
-  <autoFilter ref="A4:E72" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Tabelle1" displayName="Tabelle1" ref="A4:E69" totalsRowShown="0" dataDxfId="5">
+  <autoFilter ref="A4:E69" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
   <tableColumns count="5">
     <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Reference" dataDxfId="4"/>
     <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Value" dataDxfId="3"/>
@@ -1077,10 +1059,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A2:H76"/>
+  <dimension ref="A2:H73"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A9" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="J61" sqref="J61"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="K4" sqref="K4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1102,10 +1084,10 @@
         <v>0</v>
       </c>
       <c r="D2" s="6" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
       <c r="E2" s="7" t="s">
-        <v>217</v>
+        <v>209</v>
       </c>
     </row>
     <row r="3" spans="1:8" ht="21" x14ac:dyDescent="0.35">
@@ -1113,30 +1095,30 @@
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
+        <v>87</v>
+      </c>
+      <c r="B4" t="s">
         <v>88</v>
       </c>
-      <c r="B4" t="s">
+      <c r="C4" t="s">
         <v>89</v>
       </c>
-      <c r="C4" t="s">
+      <c r="D4" t="s">
         <v>90</v>
       </c>
-      <c r="D4" t="s">
-        <v>91</v>
-      </c>
       <c r="E4" s="3" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B5" s="3" t="s">
         <v>12</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
       <c r="D5" s="3">
         <v>1043</v>
@@ -1147,7 +1129,7 @@
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
       <c r="B6" s="3" t="s">
         <v>14</v>
@@ -1165,16 +1147,16 @@
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
       <c r="D7" s="4" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
       <c r="E7" s="5">
         <v>3</v>
@@ -1183,7 +1165,7 @@
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="B8" s="3" t="s">
         <v>19</v>
@@ -1201,7 +1183,7 @@
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="B9" s="3" t="s">
         <v>17</v>
@@ -1219,16 +1201,16 @@
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="D10" s="4" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="E10" s="5">
         <v>1</v>
@@ -1237,10 +1219,10 @@
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" s="3" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="C11" s="3" t="s">
         <v>6</v>
@@ -1255,16 +1237,16 @@
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" s="3" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C12" s="3" t="s">
-        <v>139</v>
+        <v>136</v>
       </c>
       <c r="D12" s="4" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
       <c r="E12" s="5">
         <v>2</v>
@@ -1273,10 +1255,10 @@
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" s="3" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="C13" s="3" t="s">
         <v>7</v>
@@ -1291,10 +1273,10 @@
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" s="3" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="C14" s="3" t="s">
         <v>6</v>
@@ -1312,7 +1294,7 @@
         <v>21</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>143</v>
+        <v>140</v>
       </c>
       <c r="C15" s="3" t="s">
         <v>38</v>
@@ -1330,13 +1312,13 @@
         <v>22</v>
       </c>
       <c r="B16" s="3" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
       <c r="C16" s="3" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
       <c r="D16" s="4" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
       <c r="E16" s="5">
         <v>1</v>
@@ -1351,7 +1333,7 @@
         <v>34</v>
       </c>
       <c r="C17" s="3" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
       <c r="D17" s="4" t="s">
         <v>35</v>
@@ -1363,13 +1345,13 @@
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A18" s="3" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
       <c r="B18" s="3" t="s">
         <v>31</v>
       </c>
       <c r="C18" s="3" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
       <c r="D18" s="4" t="s">
         <v>32</v>
@@ -1381,7 +1363,7 @@
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A19" s="3" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
       <c r="B19" s="3" t="s">
         <v>29</v>
@@ -1402,13 +1384,13 @@
         <v>33</v>
       </c>
       <c r="B20" s="3" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
       <c r="C20" s="3" t="s">
-        <v>147</v>
+        <v>144</v>
       </c>
       <c r="D20" s="4" t="s">
-        <v>148</v>
+        <v>145</v>
       </c>
       <c r="E20" s="5">
         <v>1</v>
@@ -1420,13 +1402,13 @@
         <v>36</v>
       </c>
       <c r="B21" s="3" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
       <c r="C21" s="3" t="s">
         <v>55</v>
       </c>
       <c r="D21" s="4" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
       <c r="E21" s="5">
         <v>1</v>
@@ -1453,13 +1435,13 @@
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A23" s="3" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
       <c r="B23" s="3" t="s">
         <v>9</v>
       </c>
       <c r="C23" s="3" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
       <c r="D23" s="4" t="s">
         <v>8</v>
@@ -1471,7 +1453,7 @@
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A24" s="3" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
       <c r="B24" s="3" t="s">
         <v>10</v>
@@ -1489,16 +1471,16 @@
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A25" s="3" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
       <c r="B25" s="3" t="s">
-        <v>154</v>
+        <v>151</v>
       </c>
       <c r="C25" s="3" t="s">
         <v>30</v>
       </c>
       <c r="D25" s="4" t="s">
-        <v>154</v>
+        <v>151</v>
       </c>
       <c r="E25" s="5">
         <v>1</v>
@@ -1525,16 +1507,16 @@
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A27" s="3" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
       <c r="B27" s="3" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="C27" s="3" t="s">
-        <v>156</v>
+        <v>153</v>
       </c>
       <c r="D27" s="4" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="E27" s="5">
         <v>1</v>
@@ -1543,16 +1525,16 @@
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A28" s="3" t="s">
+        <v>154</v>
+      </c>
+      <c r="B28" s="4" t="s">
+        <v>155</v>
+      </c>
+      <c r="C28" s="3" t="s">
+        <v>156</v>
+      </c>
+      <c r="D28" s="4" t="s">
         <v>157</v>
-      </c>
-      <c r="B28" s="4" t="s">
-        <v>158</v>
-      </c>
-      <c r="C28" s="3" t="s">
-        <v>159</v>
-      </c>
-      <c r="D28" s="4" t="s">
-        <v>160</v>
       </c>
       <c r="E28" s="5">
         <v>1</v>
@@ -1579,10 +1561,10 @@
     </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A30" s="3" t="s">
-        <v>161</v>
+        <v>158</v>
       </c>
       <c r="B30" s="3" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="C30" s="3" t="s">
         <v>47</v>
@@ -1597,7 +1579,7 @@
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A31" s="3" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
       <c r="B31" s="3" t="s">
         <v>50</v>
@@ -1606,7 +1588,7 @@
         <v>47</v>
       </c>
       <c r="D31" s="4" t="s">
-        <v>163</v>
+        <v>160</v>
       </c>
       <c r="E31" s="5">
         <v>1</v>
@@ -1633,16 +1615,16 @@
     </row>
     <row r="33" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A33" s="3" t="s">
-        <v>164</v>
+        <v>161</v>
       </c>
       <c r="B33" s="3" t="s">
-        <v>165</v>
+        <v>162</v>
       </c>
       <c r="C33" s="3" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
       <c r="D33" s="4" t="s">
-        <v>165</v>
+        <v>162</v>
       </c>
       <c r="E33" s="5">
         <v>1</v>
@@ -1669,34 +1651,34 @@
     </row>
     <row r="35" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A35" s="3" t="s">
-        <v>167</v>
+        <v>53</v>
       </c>
       <c r="B35" s="3" t="s">
-        <v>168</v>
+        <v>108</v>
       </c>
       <c r="C35" s="3" t="s">
-        <v>67</v>
+        <v>109</v>
       </c>
       <c r="D35" s="4" t="s">
-        <v>67</v>
+        <v>110</v>
       </c>
       <c r="E35" s="5">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H35" s="2"/>
     </row>
     <row r="36" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A36" s="3" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="B36" s="3" t="s">
-        <v>109</v>
+        <v>61</v>
       </c>
       <c r="C36" s="3" t="s">
-        <v>110</v>
+        <v>62</v>
       </c>
       <c r="D36" s="4" t="s">
-        <v>111</v>
+        <v>61</v>
       </c>
       <c r="E36" s="5">
         <v>1</v>
@@ -1704,154 +1686,154 @@
     </row>
     <row r="37" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A37" s="3" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="B37" s="3" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="C37" s="3" t="s">
-        <v>62</v>
+        <v>55</v>
       </c>
       <c r="D37" s="4" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="E37" s="5">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H37" s="2"/>
     </row>
     <row r="38" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A38" s="3" t="s">
-        <v>56</v>
+        <v>164</v>
       </c>
       <c r="B38" s="3" t="s">
-        <v>57</v>
+        <v>165</v>
       </c>
       <c r="C38" s="3" t="s">
-        <v>55</v>
+        <v>166</v>
       </c>
       <c r="D38" s="3" t="s">
-        <v>57</v>
+        <v>167</v>
       </c>
       <c r="E38" s="5">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H38" s="2"/>
     </row>
     <row r="39" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A39" s="3" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="B39" s="3" t="s">
-        <v>170</v>
+        <v>58</v>
       </c>
       <c r="C39" s="3" t="s">
-        <v>171</v>
+        <v>59</v>
       </c>
       <c r="D39" s="3" t="s">
-        <v>172</v>
+        <v>60</v>
       </c>
       <c r="E39" s="5">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="40" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A40" s="3" t="s">
-        <v>173</v>
+        <v>118</v>
       </c>
       <c r="B40" s="3" t="s">
-        <v>58</v>
+        <v>212</v>
       </c>
       <c r="C40" s="3" t="s">
-        <v>59</v>
+        <v>111</v>
       </c>
       <c r="D40" s="3" t="s">
-        <v>60</v>
+        <v>112</v>
       </c>
       <c r="E40" s="5">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="41" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A41" s="3" t="s">
-        <v>121</v>
+        <v>169</v>
       </c>
       <c r="B41" s="3" t="s">
-        <v>112</v>
+        <v>63</v>
       </c>
       <c r="C41" s="3" t="s">
-        <v>113</v>
+        <v>64</v>
       </c>
       <c r="D41" s="3" t="s">
-        <v>114</v>
+        <v>65</v>
       </c>
       <c r="E41" s="5">
-        <v>1</v>
+        <v>8</v>
       </c>
     </row>
     <row r="42" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A42" s="3" t="s">
-        <v>174</v>
-      </c>
-      <c r="B42" s="3" t="s">
-        <v>63</v>
+        <v>170</v>
+      </c>
+      <c r="B42" s="3">
+        <v>300</v>
       </c>
       <c r="C42" s="3" t="s">
-        <v>64</v>
+        <v>1</v>
       </c>
       <c r="D42" s="3" t="s">
-        <v>65</v>
+        <v>76</v>
       </c>
       <c r="E42" s="5">
-        <v>8</v>
+        <v>1</v>
       </c>
     </row>
     <row r="43" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A43" s="3" t="s">
-        <v>175</v>
+        <v>171</v>
       </c>
       <c r="B43" s="3">
-        <v>300</v>
+        <v>100</v>
       </c>
       <c r="C43" s="3" t="s">
-        <v>1</v>
+        <v>15</v>
       </c>
       <c r="D43" s="3" t="s">
-        <v>77</v>
+        <v>123</v>
       </c>
       <c r="E43" s="5">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="44" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A44" s="3" t="s">
-        <v>176</v>
+        <v>172</v>
       </c>
       <c r="B44" s="3">
-        <v>100</v>
+        <v>620</v>
       </c>
       <c r="C44" s="3" t="s">
-        <v>15</v>
+        <v>124</v>
       </c>
       <c r="D44" s="3" t="s">
-        <v>126</v>
+        <v>173</v>
       </c>
       <c r="E44" s="5">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="45" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A45" s="3" t="s">
-        <v>177</v>
+        <v>174</v>
       </c>
       <c r="B45" s="3">
-        <v>620</v>
+        <v>0</v>
       </c>
       <c r="C45" s="3" t="s">
-        <v>127</v>
+        <v>15</v>
       </c>
       <c r="D45" s="3" t="s">
-        <v>178</v>
+        <v>66</v>
       </c>
       <c r="E45" s="5">
         <v>3</v>
@@ -1859,50 +1841,50 @@
     </row>
     <row r="46" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A46" s="3" t="s">
-        <v>179</v>
+        <v>175</v>
       </c>
       <c r="B46" s="3">
-        <v>0</v>
+        <v>470</v>
       </c>
       <c r="C46" s="3" t="s">
-        <v>15</v>
+        <v>64</v>
       </c>
       <c r="D46" s="3" t="s">
-        <v>66</v>
+        <v>69</v>
       </c>
       <c r="E46" s="5">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="47" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A47" s="3" t="s">
-        <v>180</v>
-      </c>
-      <c r="B47" s="3">
-        <v>470</v>
+        <v>102</v>
+      </c>
+      <c r="B47" s="3" t="s">
+        <v>176</v>
       </c>
       <c r="C47" s="3" t="s">
-        <v>64</v>
+        <v>177</v>
       </c>
       <c r="D47" s="3" t="s">
-        <v>70</v>
+        <v>178</v>
       </c>
       <c r="E47" s="5">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="48" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A48" s="3" t="s">
-        <v>103</v>
+        <v>179</v>
       </c>
       <c r="B48" s="3" t="s">
+        <v>180</v>
+      </c>
+      <c r="C48" s="3" t="s">
         <v>181</v>
       </c>
-      <c r="C48" s="3" t="s">
+      <c r="D48" s="3" t="s">
         <v>182</v>
-      </c>
-      <c r="D48" s="3" t="s">
-        <v>183</v>
       </c>
       <c r="E48" s="5">
         <v>1</v>
@@ -1910,16 +1892,16 @@
     </row>
     <row r="49" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A49" s="3" t="s">
-        <v>184</v>
-      </c>
-      <c r="B49" s="3" t="s">
-        <v>185</v>
+        <v>119</v>
+      </c>
+      <c r="B49" s="3">
+        <v>0</v>
       </c>
       <c r="C49" s="3" t="s">
-        <v>186</v>
+        <v>15</v>
       </c>
       <c r="D49" s="3" t="s">
-        <v>187</v>
+        <v>94</v>
       </c>
       <c r="E49" s="5">
         <v>1</v>
@@ -1927,16 +1909,16 @@
     </row>
     <row r="50" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A50" s="3" t="s">
-        <v>122</v>
-      </c>
-      <c r="B50" s="3">
-        <v>0</v>
+        <v>183</v>
+      </c>
+      <c r="B50" s="3" t="s">
+        <v>70</v>
       </c>
       <c r="C50" s="3" t="s">
         <v>15</v>
       </c>
       <c r="D50" s="3" t="s">
-        <v>95</v>
+        <v>71</v>
       </c>
       <c r="E50" s="5">
         <v>1</v>
@@ -1944,16 +1926,16 @@
     </row>
     <row r="51" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A51" s="3" t="s">
-        <v>188</v>
+        <v>184</v>
       </c>
       <c r="B51" s="3" t="s">
-        <v>71</v>
+        <v>113</v>
       </c>
       <c r="C51" s="3" t="s">
-        <v>15</v>
+        <v>64</v>
       </c>
       <c r="D51" s="3" t="s">
-        <v>72</v>
+        <v>65</v>
       </c>
       <c r="E51" s="5">
         <v>1</v>
@@ -1961,16 +1943,16 @@
     </row>
     <row r="52" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A52" s="3" t="s">
-        <v>189</v>
+        <v>185</v>
       </c>
       <c r="B52" s="3" t="s">
-        <v>115</v>
+        <v>74</v>
       </c>
       <c r="C52" s="3" t="s">
-        <v>64</v>
+        <v>15</v>
       </c>
       <c r="D52" s="3" t="s">
-        <v>65</v>
+        <v>75</v>
       </c>
       <c r="E52" s="5">
         <v>1</v>
@@ -1978,16 +1960,16 @@
     </row>
     <row r="53" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A53" s="3" t="s">
-        <v>190</v>
+        <v>186</v>
       </c>
       <c r="B53" s="3" t="s">
-        <v>75</v>
+        <v>67</v>
       </c>
       <c r="C53" s="3" t="s">
-        <v>15</v>
+        <v>64</v>
       </c>
       <c r="D53" s="3" t="s">
-        <v>76</v>
+        <v>68</v>
       </c>
       <c r="E53" s="5">
         <v>1</v>
@@ -1995,50 +1977,50 @@
     </row>
     <row r="54" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A54" s="3" t="s">
-        <v>191</v>
+        <v>187</v>
       </c>
       <c r="B54" s="3" t="s">
-        <v>68</v>
+        <v>72</v>
       </c>
       <c r="C54" s="3" t="s">
         <v>64</v>
       </c>
       <c r="D54" s="3" t="s">
-        <v>69</v>
+        <v>73</v>
       </c>
       <c r="E54" s="5">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="55" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A55" s="3" t="s">
-        <v>192</v>
+        <v>188</v>
       </c>
       <c r="B55" s="3" t="s">
-        <v>73</v>
+        <v>189</v>
       </c>
       <c r="C55" s="3" t="s">
-        <v>64</v>
+        <v>190</v>
       </c>
       <c r="D55" s="3" t="s">
-        <v>74</v>
+        <v>191</v>
       </c>
       <c r="E55" s="5">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="56" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A56" s="3" t="s">
+        <v>192</v>
+      </c>
+      <c r="B56" s="3" t="s">
         <v>193</v>
       </c>
-      <c r="B56" s="3" t="s">
+      <c r="C56" s="3" t="s">
+        <v>190</v>
+      </c>
+      <c r="D56" s="3" t="s">
         <v>194</v>
-      </c>
-      <c r="C56" s="3" t="s">
-        <v>195</v>
-      </c>
-      <c r="D56" s="3" t="s">
-        <v>196</v>
       </c>
       <c r="E56" s="5">
         <v>1</v>
@@ -2046,16 +2028,16 @@
     </row>
     <row r="57" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A57" s="3" t="s">
+        <v>195</v>
+      </c>
+      <c r="B57" s="3" t="s">
+        <v>196</v>
+      </c>
+      <c r="C57" s="3" t="s">
         <v>197</v>
       </c>
-      <c r="B57" s="3" t="s">
+      <c r="D57" s="3" t="s">
         <v>198</v>
-      </c>
-      <c r="C57" s="3" t="s">
-        <v>195</v>
-      </c>
-      <c r="D57" s="3" t="s">
-        <v>199</v>
       </c>
       <c r="E57" s="5">
         <v>1</v>
@@ -2063,16 +2045,16 @@
     </row>
     <row r="58" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A58" s="3" t="s">
-        <v>200</v>
+        <v>77</v>
       </c>
       <c r="B58" s="3" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="C58" s="3" t="s">
-        <v>202</v>
+        <v>2</v>
       </c>
       <c r="D58" s="3" t="s">
-        <v>203</v>
+        <v>78</v>
       </c>
       <c r="E58" s="5">
         <v>1</v>
@@ -2080,50 +2062,50 @@
     </row>
     <row r="59" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A59" s="3" t="s">
-        <v>78</v>
+        <v>210</v>
       </c>
       <c r="B59" s="3" t="s">
-        <v>204</v>
+        <v>200</v>
       </c>
       <c r="C59" s="3" t="s">
-        <v>2</v>
+        <v>201</v>
       </c>
       <c r="D59" s="3" t="s">
-        <v>79</v>
+        <v>202</v>
       </c>
       <c r="E59" s="5">
-        <v>1</v>
+        <v>5</v>
       </c>
     </row>
     <row r="60" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A60" s="3" t="s">
-        <v>218</v>
+        <v>203</v>
       </c>
       <c r="B60" s="3" t="s">
-        <v>205</v>
+        <v>211</v>
       </c>
       <c r="C60" s="3" t="s">
-        <v>206</v>
+        <v>2</v>
       </c>
       <c r="D60" s="3" t="s">
-        <v>207</v>
+        <v>211</v>
       </c>
       <c r="E60" s="5">
-        <v>5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="61" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A61" s="3" t="s">
-        <v>208</v>
+        <v>79</v>
       </c>
       <c r="B61" s="3" t="s">
-        <v>219</v>
+        <v>204</v>
       </c>
       <c r="C61" s="3" t="s">
-        <v>2</v>
+        <v>205</v>
       </c>
       <c r="D61" s="3" t="s">
-        <v>219</v>
+        <v>204</v>
       </c>
       <c r="E61" s="5">
         <v>1</v>
@@ -2131,176 +2113,125 @@
     </row>
     <row r="62" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A62" s="3" t="s">
-        <v>209</v>
+        <v>82</v>
       </c>
       <c r="B62" s="3" t="s">
-        <v>210</v>
+        <v>206</v>
       </c>
       <c r="C62" s="3" t="s">
-        <v>67</v>
+        <v>207</v>
       </c>
       <c r="D62" s="3" t="s">
-        <v>67</v>
+        <v>206</v>
       </c>
       <c r="E62" s="5">
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="63" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A63" s="3" t="s">
-        <v>211</v>
+        <v>83</v>
       </c>
       <c r="B63" s="3" t="s">
-        <v>116</v>
+        <v>80</v>
       </c>
       <c r="C63" s="3" t="s">
-        <v>67</v>
+        <v>81</v>
       </c>
       <c r="D63" s="3" t="s">
-        <v>67</v>
+        <v>80</v>
       </c>
       <c r="E63" s="5">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="64" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A64" s="3" t="s">
-        <v>80</v>
+        <v>84</v>
       </c>
       <c r="B64" s="3" t="s">
-        <v>212</v>
+        <v>208</v>
       </c>
       <c r="C64" s="3" t="s">
         <v>213</v>
       </c>
       <c r="D64" s="3" t="s">
-        <v>212</v>
+        <v>208</v>
       </c>
       <c r="E64" s="5">
         <v>1</v>
       </c>
     </row>
     <row r="65" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A65" s="3" t="s">
-        <v>83</v>
-      </c>
-      <c r="B65" s="3" t="s">
-        <v>214</v>
-      </c>
-      <c r="C65" s="3" t="s">
-        <v>215</v>
-      </c>
-      <c r="D65" s="3" t="s">
-        <v>214</v>
-      </c>
-      <c r="E65" s="5">
-        <v>1</v>
-      </c>
+      <c r="A65" s="3"/>
+      <c r="B65" s="3"/>
+      <c r="C65" s="3"/>
+      <c r="D65" s="3"/>
     </row>
     <row r="66" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A66" s="3" t="s">
-        <v>84</v>
+        <v>98</v>
       </c>
       <c r="B66" s="3" t="s">
-        <v>81</v>
+        <v>96</v>
       </c>
       <c r="C66" s="3" t="s">
-        <v>82</v>
-      </c>
-      <c r="D66" s="3" t="s">
-        <v>81</v>
+        <v>97</v>
+      </c>
+      <c r="D66" s="3">
+        <v>100833</v>
       </c>
       <c r="E66" s="5">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="67" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A67" s="3" t="s">
-        <v>85</v>
+        <v>91</v>
       </c>
       <c r="B67" s="3" t="s">
-        <v>216</v>
+        <v>92</v>
       </c>
       <c r="C67" s="3" t="s">
-        <v>67</v>
+        <v>47</v>
       </c>
       <c r="D67" s="3" t="s">
-        <v>67</v>
+        <v>93</v>
       </c>
       <c r="E67" s="5">
         <v>1</v>
       </c>
     </row>
     <row r="68" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A68" s="3"/>
-      <c r="B68" s="3"/>
-      <c r="C68" s="3"/>
-      <c r="D68" s="3"/>
+      <c r="A68" s="3" t="s">
+        <v>114</v>
+      </c>
+      <c r="B68" s="3" t="s">
+        <v>115</v>
+      </c>
+      <c r="C68" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="D68" s="3" t="s">
+        <v>116</v>
+      </c>
+      <c r="E68" s="5">
+        <v>2</v>
+      </c>
     </row>
     <row r="69" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A69" s="3" t="s">
-        <v>99</v>
-      </c>
-      <c r="B69" s="3" t="s">
-        <v>97</v>
-      </c>
-      <c r="C69" s="3" t="s">
-        <v>98</v>
-      </c>
-      <c r="D69" s="3">
-        <v>100833</v>
-      </c>
-      <c r="E69" s="5">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="70" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A70" s="3" t="s">
-        <v>92</v>
-      </c>
-      <c r="B70" s="3" t="s">
-        <v>93</v>
-      </c>
-      <c r="C70" s="3" t="s">
-        <v>47</v>
-      </c>
-      <c r="D70" s="3" t="s">
-        <v>94</v>
-      </c>
-      <c r="E70" s="5">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="71" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A71" s="3" t="s">
-        <v>117</v>
-      </c>
-      <c r="B71" s="3" t="s">
-        <v>118</v>
-      </c>
-      <c r="C71" s="3" t="s">
-        <v>47</v>
-      </c>
-      <c r="D71" s="3" t="s">
-        <v>119</v>
-      </c>
-      <c r="E71" s="5">
-        <v>2</v>
-      </c>
+      <c r="A69" s="3"/>
+      <c r="B69" s="3"/>
+      <c r="C69" s="3"/>
+      <c r="D69" s="3"/>
     </row>
     <row r="72" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A72" s="3"/>
-      <c r="B72" s="3"/>
-      <c r="C72" s="3"/>
       <c r="D72" s="3"/>
     </row>
-    <row r="75" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="D75" s="3"/>
-    </row>
-    <row r="76" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A76" s="3"/>
-      <c r="B76" s="3"/>
-      <c r="C76" s="3"/>
+    <row r="73" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A73" s="3"/>
+      <c r="B73" s="3"/>
+      <c r="C73" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>

</xml_diff>